<commit_message>
adjustment to visual of network
</commit_message>
<xml_diff>
--- a/data/ecopath/nodes_statstab_UTL.xlsx
+++ b/data/ecopath/nodes_statstab_UTL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greig\Documents\GitHub\Ecosystem-Model-Data-Framework\data\ecopath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B7423D-735F-4C91-9098-A96F61715E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1A5EBE-5D95-4CAD-B177-F6018CCD5EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4100" yWindow="4100" windowWidth="16920" windowHeight="10450" xr2:uid="{17ACD660-A85B-43E8-83BF-D3DAAF979879}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{17ACD660-A85B-43E8-83BF-D3DAAF979879}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes_statstab_UTL" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="217">
   <si>
     <t>ID</t>
   </si>
@@ -642,6 +642,48 @@
   </si>
   <si>
     <t>SFf</t>
+  </si>
+  <si>
+    <t>Humpback</t>
+  </si>
+  <si>
+    <t>HPB</t>
+  </si>
+  <si>
+    <t>Lingcod</t>
+  </si>
+  <si>
+    <t>Dogfish</t>
+  </si>
+  <si>
+    <t>LNC</t>
+  </si>
+  <si>
+    <t>DGF</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>BH1-ZOS</t>
+  </si>
+  <si>
+    <t>BH2-KEL</t>
+  </si>
+  <si>
+    <t>ZOS</t>
+  </si>
+  <si>
+    <t>KEL</t>
+  </si>
+  <si>
+    <t>BH</t>
+  </si>
+  <si>
+    <t>bhab</t>
   </si>
 </sst>
 </file>
@@ -1509,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FB3787-CF9B-4BAA-9BF8-DA520FCC58E2}">
-  <dimension ref="A1:Z71"/>
+  <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N32" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1688,10 +1730,10 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O5" t="s">
-        <v>58</v>
+        <v>203</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>61</v>
+        <v>204</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>88</v>
@@ -1703,71 +1745,71 @@
         <v>1</v>
       </c>
       <c r="T5" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="U5" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="W5">
-        <v>0.08</v>
+      <c r="W5" s="1">
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="X5" s="1">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
       <c r="Y5" s="3">
-        <v>3.8</v>
-      </c>
-      <c r="Z5">
-        <v>20</v>
+        <v>3.7</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>7.3</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O6" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S6" s="1">
         <v>1</v>
       </c>
       <c r="T6" s="1">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="U6" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="W6">
-        <v>4.3999999999999997E-2</v>
+        <v>0.08</v>
       </c>
       <c r="X6" s="1">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="Y6" s="3">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="Z6">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>89</v>
@@ -1779,112 +1821,112 @@
         <v>1</v>
       </c>
       <c r="T7" s="1">
+        <v>18</v>
+      </c>
+      <c r="U7" s="1">
         <v>6</v>
-      </c>
-      <c r="U7" s="1">
-        <v>2</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>106</v>
       </c>
       <c r="W7">
-        <v>0.16</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="X7" s="1">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="Y7" s="3">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="Z7">
-        <v>14.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S8" s="1">
         <v>1</v>
       </c>
       <c r="T8" s="1">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="U8" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="W8">
-        <v>3.5999999999999997E-2</v>
+        <v>0.16</v>
       </c>
       <c r="X8" s="1">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="Y8" s="3">
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="Z8">
-        <v>124</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S9" s="1">
         <v>1</v>
       </c>
       <c r="T9" s="1">
-        <v>16.5</v>
+        <v>7.5</v>
       </c>
       <c r="U9" s="1">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="W9">
-        <v>0.30990000000000001</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="X9" s="1">
-        <v>1.7</v>
+        <v>0.15</v>
       </c>
       <c r="Y9" s="3">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="Z9">
-        <v>10.5</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O10" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>66</v>
+        <v>207</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>91</v>
+        <v>210</v>
       </c>
       <c r="R10" s="1">
         <v>5</v>
@@ -1893,457 +1935,457 @@
         <v>1</v>
       </c>
       <c r="T10" s="1">
-        <v>19.5</v>
+        <v>7.5</v>
       </c>
       <c r="U10" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W10">
-        <v>2.2669999999999999</v>
+      <c r="W10" s="1">
+        <v>1.1000000000000001</v>
       </c>
       <c r="X10" s="1">
-        <v>0.95</v>
+        <v>0.26</v>
       </c>
       <c r="Y10" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="Z10">
-        <v>4.7</v>
+        <v>2.6</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>2.4</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O11" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>67</v>
+        <v>208</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>91</v>
+        <v>209</v>
       </c>
       <c r="R11" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S11" s="1">
         <v>1</v>
       </c>
       <c r="T11" s="1">
-        <v>22.5</v>
+        <v>7.5</v>
       </c>
       <c r="U11" s="1">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W11">
-        <v>1.9</v>
+      <c r="W11" s="1">
+        <v>5</v>
       </c>
       <c r="X11" s="1">
-        <v>0.3</v>
+        <v>0.13</v>
       </c>
       <c r="Y11" s="3">
         <v>3.6</v>
       </c>
-      <c r="Z11">
-        <v>3.2</v>
+      <c r="Z11" s="1">
+        <v>2.7</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O12" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>91</v>
       </c>
       <c r="R12" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S12" s="1">
         <v>1</v>
       </c>
       <c r="T12" s="1">
-        <v>25.5</v>
+        <v>16.5</v>
       </c>
       <c r="U12" s="1">
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W12">
-        <v>4.4493</v>
+        <v>0.30990000000000001</v>
       </c>
       <c r="X12" s="1">
-        <v>0.24</v>
+        <v>1.7</v>
       </c>
       <c r="Y12" s="3">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="Z12">
-        <v>2.7</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R13" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S13" s="1">
         <v>1</v>
       </c>
       <c r="T13" s="1">
-        <v>9</v>
+        <v>19.5</v>
       </c>
       <c r="U13" s="1">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="V13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W13">
-        <v>3.3999999999999998E-3</v>
+        <v>2.2669999999999999</v>
       </c>
       <c r="X13" s="1">
-        <v>13.2</v>
+        <v>0.95</v>
       </c>
       <c r="Y13" s="3">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="Z13">
-        <v>44</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R14" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S14" s="1">
         <v>1</v>
       </c>
       <c r="T14" s="1">
-        <v>13.5</v>
+        <v>22.5</v>
       </c>
       <c r="U14" s="1">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W14">
-        <v>0.18</v>
+        <v>1.9</v>
       </c>
       <c r="X14" s="1">
-        <v>3.45</v>
+        <v>0.3</v>
       </c>
       <c r="Y14" s="3">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="Z14">
-        <v>13.4</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O15" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R15" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S15" s="1">
         <v>1</v>
       </c>
       <c r="T15" s="1">
-        <v>15</v>
+        <v>25.5</v>
       </c>
       <c r="U15" s="1">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W15">
-        <v>3.3E-3</v>
+        <v>4.4493</v>
       </c>
       <c r="X15" s="1">
-        <v>13.75</v>
+        <v>0.24</v>
       </c>
       <c r="Y15" s="3">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="Z15">
-        <v>45.8</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R16" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S16" s="1">
         <v>1</v>
       </c>
       <c r="T16" s="1">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="U16" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="V16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W16">
-        <v>0.14000000000000001</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="X16" s="1">
-        <v>1.32</v>
+        <v>13.2</v>
       </c>
       <c r="Y16" s="3">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="Z16">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R17" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S17" s="1">
         <v>1</v>
       </c>
       <c r="T17" s="1">
-        <v>21</v>
+        <v>13.5</v>
       </c>
       <c r="U17" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W17">
-        <v>6.6E-3</v>
+        <v>0.18</v>
       </c>
       <c r="X17" s="1">
-        <v>11.1</v>
+        <v>3.45</v>
       </c>
       <c r="Y17" s="3">
         <v>3.8</v>
       </c>
       <c r="Z17">
-        <v>37</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="18" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R18" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S18" s="1">
         <v>1</v>
       </c>
       <c r="T18" s="1">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U18" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W18">
-        <v>0.18</v>
+        <v>3.3E-3</v>
       </c>
       <c r="X18" s="1">
-        <v>1.37</v>
+        <v>13.75</v>
       </c>
       <c r="Y18" s="3">
         <v>3.7</v>
       </c>
       <c r="Z18">
-        <v>7</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="19" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R19" s="1">
+        <v>8</v>
+      </c>
+      <c r="S19" s="1">
+        <v>1</v>
+      </c>
+      <c r="T19" s="1">
+        <v>18</v>
+      </c>
+      <c r="U19" s="1">
         <v>6</v>
-      </c>
-      <c r="S19" s="1">
-        <v>1</v>
-      </c>
-      <c r="T19" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="U19" s="1">
-        <v>2</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W19" s="2">
-        <v>1E-4</v>
+      <c r="W19">
+        <v>0.14000000000000001</v>
       </c>
       <c r="X19" s="1">
-        <v>2.5</v>
+        <v>1.32</v>
       </c>
       <c r="Y19" s="3">
-        <v>3</v>
+        <v>3.7</v>
       </c>
       <c r="Z19">
-        <v>31.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R20" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S20" s="1">
         <v>1</v>
       </c>
       <c r="T20" s="1">
-        <v>7.5</v>
+        <v>21</v>
       </c>
       <c r="U20" s="1">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W20">
-        <v>2.0000000000000001E-4</v>
+        <v>6.6E-3</v>
       </c>
       <c r="X20" s="1">
-        <v>0.8</v>
+        <v>11.1</v>
       </c>
       <c r="Y20" s="3">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="Z20">
-        <v>18.3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O21" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R21" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S21" s="1">
         <v>1</v>
       </c>
       <c r="T21" s="1">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="U21" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W21">
-        <v>1.1000000000000001E-3</v>
+        <v>0.18</v>
       </c>
       <c r="X21" s="1">
-        <v>0.7</v>
+        <v>1.37</v>
       </c>
       <c r="Y21" s="3">
-        <v>3.2</v>
+        <v>3.7</v>
       </c>
       <c r="Z21">
-        <v>12.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O22" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R22" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S22" s="1">
         <v>1</v>
@@ -2357,31 +2399,31 @@
       <c r="V22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W22">
-        <v>1.8E-3</v>
+      <c r="W22" s="2">
+        <v>1E-4</v>
       </c>
       <c r="X22" s="1">
-        <v>0.3</v>
+        <v>2.5</v>
       </c>
       <c r="Y22" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z22">
-        <v>9</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="23" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O23" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R23" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S23" s="1">
         <v>1</v>
@@ -2396,144 +2438,144 @@
         <v>14</v>
       </c>
       <c r="W23">
-        <v>3.4599999999999999E-2</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="X23" s="1">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="Y23" s="3">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="Z23">
-        <v>5</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="24" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R24" s="1">
+        <v>8</v>
+      </c>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24" s="1">
         <v>6</v>
       </c>
-      <c r="S24" s="1">
-        <v>1</v>
-      </c>
-      <c r="T24" s="1">
-        <v>13.5</v>
-      </c>
       <c r="U24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W24">
-        <v>3.5499999999999997E-2</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="X24" s="1">
-        <v>0.89</v>
+        <v>0.7</v>
       </c>
       <c r="Y24" s="3">
         <v>3.2</v>
       </c>
       <c r="Z24">
-        <v>3.1</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="25" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O25" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R25" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S25" s="1">
         <v>1</v>
       </c>
       <c r="T25" s="1">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="U25" s="1">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W25" s="2">
-        <v>1E-4</v>
+      <c r="W25">
+        <v>1.8E-3</v>
       </c>
       <c r="X25" s="1">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="Y25" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z25">
-        <v>33.6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O26" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R26" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S26" s="1">
         <v>1</v>
       </c>
       <c r="T26" s="1">
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="U26" s="1">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="V26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W26">
-        <v>1.6000000000000001E-3</v>
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="X26" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="Y26" s="3">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="Z26">
-        <v>12.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O27" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R27" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S27" s="1">
         <v>1</v>
@@ -2542,905 +2584,869 @@
         <v>13.5</v>
       </c>
       <c r="U27" s="1">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="V27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W27">
-        <v>2.5100000000000001E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="X27" s="1">
-        <v>0.7</v>
+        <v>0.89</v>
       </c>
       <c r="Y27" s="3">
         <v>3.2</v>
       </c>
       <c r="Z27">
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="28" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O28" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R28" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S28" s="1">
         <v>1</v>
       </c>
       <c r="T28" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="U28" s="1">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="V28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W28">
-        <v>5.91E-2</v>
+      <c r="W28" s="2">
+        <v>1E-4</v>
       </c>
       <c r="X28" s="1">
-        <v>0.3</v>
+        <v>2.5</v>
       </c>
       <c r="Y28" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z28">
-        <v>4</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="29" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R29" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S29" s="1">
         <v>1</v>
       </c>
       <c r="T29" s="1">
-        <v>16.5</v>
+        <v>12</v>
       </c>
       <c r="U29" s="1">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="V29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W29">
-        <v>1.8213999999999999</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="X29" s="1">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="Y29" s="3">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="Z29">
-        <v>1.9</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="30" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O30" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R30" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S30" s="1">
         <v>1</v>
       </c>
       <c r="T30" s="1">
-        <v>19.5</v>
+        <v>13.5</v>
       </c>
       <c r="U30" s="1">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="V30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W30">
-        <v>0.9607</v>
+        <v>2.5100000000000001E-2</v>
       </c>
       <c r="X30" s="1">
-        <v>0.89</v>
+        <v>0.7</v>
       </c>
       <c r="Y30" s="3">
         <v>3.2</v>
       </c>
       <c r="Z30">
-        <v>1.2</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="31" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O31" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R31" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S31" s="1">
         <v>1</v>
       </c>
       <c r="T31" s="1">
-        <v>19.5</v>
+        <v>15</v>
       </c>
       <c r="U31" s="1">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="V31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W31">
-        <v>1.0170999999999999</v>
+        <v>5.91E-2</v>
       </c>
       <c r="X31" s="1">
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="Y31" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z31">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O32" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R32" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S32" s="1">
         <v>1</v>
       </c>
       <c r="T32" s="1">
-        <v>22.5</v>
+        <v>16.5</v>
       </c>
       <c r="U32" s="1">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="V32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W32">
-        <v>9.9000000000000008E-3</v>
+        <v>1.8213999999999999</v>
       </c>
       <c r="X32" s="1">
-        <v>2.2999999999999998</v>
+        <v>0.85</v>
       </c>
       <c r="Y32" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z32">
-        <v>13.3</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="33" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O33" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R33" s="1">
+        <v>8</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1</v>
+      </c>
+      <c r="T33" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="U33" s="1">
         <v>6</v>
-      </c>
-      <c r="S33" s="1">
-        <v>1</v>
-      </c>
-      <c r="T33" s="1">
-        <v>22.5</v>
-      </c>
-      <c r="U33" s="1">
-        <v>7.5</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W33">
-        <v>2.8000000000000001E-2</v>
+        <v>0.9607</v>
       </c>
       <c r="X33" s="1">
-        <v>1.65</v>
+        <v>0.89</v>
       </c>
       <c r="Y33" s="3">
         <v>3.2</v>
       </c>
       <c r="Z33">
-        <v>6.2</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="34" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O34" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R34" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S34" s="1">
         <v>1</v>
       </c>
       <c r="T34" s="1">
-        <v>22.5</v>
+        <v>19.5</v>
       </c>
       <c r="U34" s="1">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W34">
-        <v>5.8599999999999999E-2</v>
+        <v>1.0170999999999999</v>
       </c>
       <c r="X34" s="1">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y34" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z34">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O35" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R35" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S35" s="1">
         <v>1</v>
       </c>
       <c r="T35" s="1">
-        <v>25.5</v>
+        <v>22.5</v>
       </c>
       <c r="U35" s="1">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="V35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W35">
-        <v>2.3800000000000002E-2</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="X35" s="1">
-        <v>0.85</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Y35" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z35">
-        <v>2.6</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="36" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O36" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R36" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S36" s="1">
         <v>1</v>
       </c>
       <c r="T36" s="1">
-        <v>25.5</v>
+        <v>22.5</v>
       </c>
       <c r="U36" s="1">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="V36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W36">
-        <v>1.83E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="X36" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.65</v>
       </c>
       <c r="Y36" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z36">
-        <v>2.2000000000000002</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="37" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O37" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R37" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S37" s="1">
         <v>1</v>
       </c>
       <c r="T37" s="1">
-        <v>6</v>
+        <v>22.5</v>
       </c>
       <c r="U37" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W37" s="2">
-        <v>4.0000000000000003E-5</v>
+      <c r="W37">
+        <v>5.8599999999999999E-2</v>
       </c>
       <c r="X37" s="1">
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="Y37" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z37">
-        <v>8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="38" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O38" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R38" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S38" s="1">
         <v>1</v>
       </c>
       <c r="T38" s="1">
-        <v>6</v>
+        <v>25.5</v>
       </c>
       <c r="U38" s="1">
-        <v>2</v>
+        <v>8.5</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W38">
-        <v>1E-4</v>
+        <v>2.3800000000000002E-2</v>
       </c>
       <c r="X38" s="1">
-        <v>1.1000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="Y38" s="3">
         <v>3.2</v>
       </c>
       <c r="Z38">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="39" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O39" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R39" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S39" s="1">
         <v>1</v>
       </c>
       <c r="T39" s="1">
-        <v>10.5</v>
+        <v>25.5</v>
       </c>
       <c r="U39" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W39">
-        <v>2.0000000000000001E-4</v>
+        <v>1.83E-2</v>
       </c>
       <c r="X39" s="1">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y39" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z39">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="40" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O40" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R40" s="1">
+        <v>8</v>
+      </c>
+      <c r="S40" s="1">
+        <v>1</v>
+      </c>
+      <c r="T40" s="1">
         <v>6</v>
       </c>
-      <c r="S40" s="1">
-        <v>1</v>
-      </c>
-      <c r="T40" s="1">
-        <v>12</v>
-      </c>
       <c r="U40" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W40">
-        <v>5.0000000000000001E-4</v>
+      <c r="W40" s="2">
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="X40" s="1">
-        <v>0.85</v>
+        <v>2.4</v>
       </c>
       <c r="Y40" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z40">
-        <v>1.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O41" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R41" s="1">
+        <v>8</v>
+      </c>
+      <c r="S41" s="1">
+        <v>1</v>
+      </c>
+      <c r="T41" s="1">
         <v>6</v>
       </c>
-      <c r="S41" s="1">
-        <v>1</v>
-      </c>
-      <c r="T41" s="1">
-        <v>15</v>
-      </c>
       <c r="U41" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W41">
-        <v>5.5100000000000003E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="X41" s="1">
-        <v>3.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y41" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z41">
-        <v>8.5</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="42" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O42" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R42" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S42" s="1">
         <v>1</v>
       </c>
       <c r="T42" s="1">
-        <v>18</v>
+        <v>10.5</v>
       </c>
       <c r="U42" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="V42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W42">
-        <v>8.5000000000000006E-2</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="X42" s="1">
-        <v>1.54</v>
+        <v>0.8</v>
       </c>
       <c r="Y42" s="3">
         <v>3.2</v>
       </c>
       <c r="Z42">
-        <v>3.6</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="43" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O43" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R43" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S43" s="1">
         <v>1</v>
       </c>
       <c r="T43" s="1">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="U43" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="V43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W43">
-        <v>8.48E-2</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="X43" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="Y43" s="3">
         <v>3.2</v>
       </c>
       <c r="Z43">
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="44" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O44" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R44" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S44" s="1">
         <v>1</v>
       </c>
       <c r="T44" s="1">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U44" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W44">
-        <v>3.9E-2</v>
+        <v>5.5100000000000003E-2</v>
       </c>
       <c r="X44" s="1">
-        <v>0.85</v>
+        <v>3.9</v>
       </c>
       <c r="Y44" s="3">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Z44">
-        <v>2</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="45" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O45" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>92</v>
       </c>
       <c r="R45" s="1">
+        <v>8</v>
+      </c>
+      <c r="S45" s="1">
+        <v>1</v>
+      </c>
+      <c r="T45" s="1">
+        <v>18</v>
+      </c>
+      <c r="U45" s="1">
         <v>6</v>
-      </c>
-      <c r="S45" s="1">
-        <v>1</v>
-      </c>
-      <c r="T45" s="1">
-        <v>27</v>
-      </c>
-      <c r="U45" s="1">
-        <v>9</v>
       </c>
       <c r="V45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W45">
-        <v>7.0499999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="X45" s="1">
-        <v>1.4</v>
+        <v>1.54</v>
       </c>
       <c r="Y45" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="Z45">
-        <v>1.7</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="46" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O46" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>75</v>
+        <v>173</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R46" s="1">
+        <v>8</v>
+      </c>
+      <c r="S46" s="1">
+        <v>1</v>
+      </c>
+      <c r="T46" s="1">
+        <v>21</v>
+      </c>
+      <c r="U46" s="1">
         <v>7</v>
-      </c>
-      <c r="S46" s="1">
-        <v>1</v>
-      </c>
-      <c r="T46" s="1">
-        <v>15</v>
-      </c>
-      <c r="U46" s="1">
-        <v>5</v>
       </c>
       <c r="V46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W46">
-        <v>0.58020000000000005</v>
+        <v>8.48E-2</v>
       </c>
       <c r="X46" s="1">
-        <v>1.75</v>
+        <v>0.8</v>
       </c>
       <c r="Y46" s="3">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="Z46">
-        <v>9</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="47" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O47" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>76</v>
+        <v>175</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R47" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S47" s="1">
         <v>1</v>
       </c>
       <c r="T47" s="1">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="U47" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W47">
-        <v>5.8887</v>
+        <v>3.9E-2</v>
       </c>
       <c r="X47" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="Y47" s="3">
         <v>3.2</v>
       </c>
       <c r="Z47">
-        <v>3.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="15:26" x14ac:dyDescent="0.35">
       <c r="O48" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R48" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S48" s="1">
         <v>1</v>
       </c>
       <c r="T48" s="1">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="U48" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="V48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W48">
-        <v>12</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="X48" s="1">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="Y48" s="3">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="Z48">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="O49" t="s">
-        <v>51</v>
+        <v>178</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R49" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S49" s="1">
         <v>1</v>
       </c>
       <c r="T49" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U49" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W49">
-        <v>26</v>
+        <v>0.58020000000000005</v>
       </c>
       <c r="X49" s="1">
-        <v>3</v>
+        <v>1.75</v>
       </c>
       <c r="Y49" s="3">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="Z49">
-        <v>7.6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>181</v>
-      </c>
-      <c r="C50" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <v>8</v>
-      </c>
-      <c r="G50">
-        <v>10</v>
-      </c>
-      <c r="H50">
-        <v>5</v>
-      </c>
-      <c r="I50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50">
-        <v>0.12</v>
-      </c>
-      <c r="K50">
-        <v>6.1</v>
-      </c>
-      <c r="L50">
-        <v>4.0999999999999996</v>
-      </c>
       <c r="O50" t="s">
-        <v>52</v>
+        <v>179</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>202</v>
+        <v>76</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R50" s="1">
         <v>9</v>
@@ -3449,152 +3455,80 @@
         <v>1</v>
       </c>
       <c r="T50" s="1">
-        <v>11.100000000000001</v>
+        <v>9</v>
       </c>
       <c r="U50" s="1">
-        <v>3.7</v>
+        <v>3</v>
       </c>
       <c r="V50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W50">
-        <v>17.5</v>
+        <v>5.8887</v>
       </c>
       <c r="X50" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="Y50" s="3">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="Z50">
-        <v>7.6</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A51">
+      <c r="O51" t="s">
+        <v>180</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R51" s="1">
+        <v>9</v>
+      </c>
+      <c r="S51" s="1">
+        <v>1</v>
+      </c>
+      <c r="T51" s="1">
+        <v>6</v>
+      </c>
+      <c r="U51" s="1">
         <v>2</v>
-      </c>
-      <c r="B51" t="s">
-        <v>182</v>
-      </c>
-      <c r="C51" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
-        <v>8.4</v>
-      </c>
-      <c r="G51">
-        <v>9</v>
-      </c>
-      <c r="H51">
-        <v>4</v>
-      </c>
-      <c r="I51" t="s">
-        <v>14</v>
-      </c>
-      <c r="J51">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="K51">
-        <v>7.2</v>
-      </c>
-      <c r="L51">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O51" t="s">
-        <v>183</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R51" s="1">
-        <v>10</v>
-      </c>
-      <c r="S51" s="1">
-        <v>7</v>
-      </c>
-      <c r="T51" s="1">
-        <v>12</v>
-      </c>
-      <c r="U51" s="1">
-        <v>4</v>
       </c>
       <c r="V51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="W51">
-        <v>1.3</v>
+        <v>12</v>
       </c>
       <c r="X51" s="1">
-        <v>3.7</v>
+        <v>0.5</v>
       </c>
       <c r="Y51" s="3">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="Z51">
-        <v>12.3</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>3</v>
-      </c>
-      <c r="B52" t="s">
-        <v>184</v>
-      </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G52">
-        <v>8</v>
-      </c>
-      <c r="H52">
-        <v>3.7</v>
-      </c>
-      <c r="I52" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52">
-        <v>3</v>
-      </c>
-      <c r="K52">
-        <v>4</v>
-      </c>
-      <c r="L52">
-        <v>3.5</v>
-      </c>
       <c r="O52" t="s">
-        <v>185</v>
+        <v>51</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="R52" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S52" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="T52" s="1">
         <v>6</v>
@@ -3603,326 +3537,326 @@
         <v>2</v>
       </c>
       <c r="V52" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="W52">
-        <v>11.7</v>
+        <v>26</v>
       </c>
       <c r="X52" s="1">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="Y52" s="3">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="Z52">
-        <v>23.2</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G53">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J53">
-        <v>1.3</v>
+        <v>0.12</v>
       </c>
       <c r="K53">
-        <v>3.7</v>
+        <v>6.1</v>
       </c>
       <c r="L53">
-        <v>2.8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O53" t="s">
-        <v>186</v>
+        <v>52</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>23</v>
+        <v>202</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="R53" s="1">
         <v>11</v>
       </c>
       <c r="S53" s="1">
-        <v>6.2</v>
+        <v>1</v>
       </c>
       <c r="T53" s="1">
-        <v>14.100000000000001</v>
+        <v>11.100000000000001</v>
       </c>
       <c r="U53" s="1">
-        <v>4.7</v>
+        <v>3.7</v>
       </c>
       <c r="V53" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="W53">
-        <v>4.8</v>
+        <v>17.5</v>
       </c>
       <c r="X53" s="1">
-        <v>7.8</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y53" s="3">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="Z53">
-        <v>26</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C54" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F54">
-        <v>6</v>
+        <v>8.4</v>
       </c>
       <c r="G54">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I54" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J54">
-        <v>10.5</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K54">
-        <v>6</v>
+        <v>7.2</v>
       </c>
       <c r="L54">
-        <v>2.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O54" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R54" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S54" s="1">
-        <v>6.4</v>
+        <v>7</v>
       </c>
       <c r="T54" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="U54" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="W54">
-        <v>2.6</v>
+        <v>1.3</v>
       </c>
       <c r="X54" s="1">
-        <v>5.7</v>
+        <v>3.7</v>
       </c>
       <c r="Y54" s="3">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="Z54">
-        <v>21.9</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G55">
+        <v>8</v>
+      </c>
+      <c r="H55">
+        <v>3.7</v>
+      </c>
+      <c r="I55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55">
         <v>3</v>
       </c>
-      <c r="F55">
-        <v>6.2</v>
-      </c>
-      <c r="G55">
-        <v>7</v>
-      </c>
-      <c r="H55">
-        <v>4.7</v>
-      </c>
-      <c r="I55" t="s">
-        <v>22</v>
-      </c>
-      <c r="J55">
-        <v>4.8</v>
-      </c>
       <c r="K55">
-        <v>7.8</v>
+        <v>4</v>
       </c>
       <c r="L55">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O55" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>21</v>
       </c>
       <c r="R55" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S55" s="1">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="T55" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="U55" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="W55">
-        <v>8</v>
+        <v>11.7</v>
       </c>
       <c r="X55" s="1">
-        <v>8.85</v>
+        <v>6.5</v>
       </c>
       <c r="Y55" s="3">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="Z55">
-        <v>31.6</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
         <v>7</v>
       </c>
-      <c r="B56" t="s">
-        <v>187</v>
-      </c>
-      <c r="C56" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" t="s">
-        <v>21</v>
-      </c>
-      <c r="E56">
-        <v>3</v>
-      </c>
-      <c r="F56">
-        <v>6.4</v>
-      </c>
       <c r="G56">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H56">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I56" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J56">
-        <v>2.6</v>
+        <v>1.3</v>
       </c>
       <c r="K56">
-        <v>5.7</v>
+        <v>3.7</v>
       </c>
       <c r="L56">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="O56" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>21</v>
       </c>
       <c r="R56" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S56" s="1">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="T56" s="1">
-        <v>15</v>
+        <v>14.100000000000001</v>
       </c>
       <c r="U56" s="1">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="V56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="W56">
-        <v>12.1</v>
+        <v>4.8</v>
       </c>
       <c r="X56" s="1">
-        <v>16.5</v>
+        <v>7.8</v>
       </c>
       <c r="Y56" s="3">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="Z56">
-        <v>58.9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
         <v>21</v>
@@ -3931,72 +3865,72 @@
         <v>3</v>
       </c>
       <c r="F57">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I57" t="s">
         <v>22</v>
       </c>
       <c r="J57">
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="K57">
-        <v>8.8000000000000007</v>
+        <v>6</v>
       </c>
       <c r="L57">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="O57" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="R57" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S57" s="1">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="T57" s="1">
-        <v>19.200000000000003</v>
+        <v>9</v>
       </c>
       <c r="U57" s="1">
-        <v>6.4</v>
+        <v>3</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="W57">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="X57" s="1">
-        <v>6.7</v>
+        <v>5.7</v>
       </c>
       <c r="Y57" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="Z57">
-        <v>8.9</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D58" t="s">
         <v>21</v>
@@ -4005,294 +3939,294 @@
         <v>3</v>
       </c>
       <c r="F58">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="G58">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H58">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="I58" t="s">
         <v>22</v>
       </c>
       <c r="J58">
-        <v>12.1</v>
+        <v>4.8</v>
       </c>
       <c r="K58">
-        <v>16.5</v>
+        <v>7.8</v>
       </c>
       <c r="L58">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="O58" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="R58" s="1">
+        <v>13</v>
+      </c>
+      <c r="S58" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="T58" s="1">
         <v>12</v>
       </c>
-      <c r="S58" s="1">
-        <v>5.2</v>
-      </c>
-      <c r="T58" s="1">
-        <v>18</v>
-      </c>
       <c r="U58" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="W58">
-        <v>9.8000000000000007</v>
+        <v>8</v>
       </c>
       <c r="X58" s="1">
-        <v>20</v>
+        <v>8.85</v>
       </c>
       <c r="Y58" s="3">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="Z58">
-        <v>26.7</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D59" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59">
-        <v>5</v>
+        <v>6.4</v>
       </c>
       <c r="G59">
         <v>6</v>
       </c>
       <c r="H59">
-        <v>6.4</v>
+        <v>3</v>
       </c>
       <c r="I59" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J59">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="K59">
-        <v>6.7</v>
+        <v>5.7</v>
       </c>
       <c r="L59">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="O59" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="R59" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S59" s="1">
-        <v>5.4</v>
+        <v>6.8</v>
       </c>
       <c r="T59" s="1">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="U59" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="W59">
-        <v>6.8</v>
+        <v>12.1</v>
       </c>
       <c r="X59" s="1">
-        <v>5</v>
+        <v>16.5</v>
       </c>
       <c r="Y59" s="3">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="Z59">
-        <v>13.9</v>
+        <v>58.9</v>
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D60" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60">
-        <v>5.2</v>
+        <v>6.6</v>
       </c>
       <c r="G60">
         <v>5</v>
       </c>
       <c r="H60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I60" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J60">
-        <v>9.8000000000000007</v>
+        <v>8</v>
       </c>
       <c r="K60">
-        <v>20</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L60">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O60" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Q60" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R60" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="S60" s="1">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="T60" s="1">
-        <v>21</v>
+        <v>19.200000000000003</v>
       </c>
       <c r="U60" s="1">
-        <v>7</v>
+        <v>6.4</v>
       </c>
       <c r="V60" s="1" t="s">
         <v>101</v>
       </c>
       <c r="W60">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="X60" s="1">
-        <v>90</v>
+        <v>6.7</v>
       </c>
       <c r="Y60" s="3">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="Z60">
-        <v>128.6</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61">
-        <v>5.4</v>
+        <v>6.8</v>
       </c>
       <c r="G61">
         <v>4</v>
       </c>
       <c r="H61">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I61" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J61">
-        <v>6.8</v>
+        <v>12.1</v>
       </c>
       <c r="K61">
-        <v>5</v>
+        <v>16.5</v>
       </c>
       <c r="L61">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="O61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R61" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S61" s="1">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="T61" s="1">
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="U61" s="1">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="V61" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W61">
-        <v>9</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="X61" s="1">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="Y61" s="3">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="Z61">
-        <v>257.10000000000002</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C62" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
         <v>28</v>
@@ -4301,644 +4235,647 @@
         <v>4</v>
       </c>
       <c r="F62">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="G62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H62">
-        <v>7</v>
+        <v>6.4</v>
       </c>
       <c r="I62" t="s">
         <v>29</v>
       </c>
       <c r="J62">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="K62">
-        <v>90</v>
+        <v>6.7</v>
       </c>
       <c r="L62">
-        <v>2.2999999999999998</v>
+        <v>3.5</v>
       </c>
       <c r="O62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R62" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S62" s="1">
-        <v>4.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="T62" s="1">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="U62" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V62" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W62">
-        <v>10</v>
+        <v>6.8</v>
       </c>
       <c r="X62" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="Y62" s="3">
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="Z62">
-        <v>156.30000000000001</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <v>5.2</v>
+      </c>
+      <c r="G63">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>6</v>
+      </c>
+      <c r="I63" t="s">
+        <v>29</v>
+      </c>
+      <c r="J63">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K63">
+        <v>20</v>
+      </c>
+      <c r="L63">
+        <v>3.1</v>
+      </c>
+      <c r="O63" t="s">
+        <v>193</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R63" s="1">
         <v>14</v>
       </c>
-      <c r="B63" t="s">
-        <v>194</v>
-      </c>
-      <c r="C63" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63">
-        <v>5</v>
-      </c>
-      <c r="F63">
-        <v>4</v>
-      </c>
-      <c r="G63">
-        <v>4</v>
-      </c>
-      <c r="H63">
-        <v>5.5</v>
-      </c>
-      <c r="I63" t="s">
-        <v>35</v>
-      </c>
-      <c r="J63">
-        <v>9.5</v>
-      </c>
-      <c r="K63">
+      <c r="S63" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="T63" s="1">
+        <v>21</v>
+      </c>
+      <c r="U63" s="1">
+        <v>7</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W63">
+        <v>3.3</v>
+      </c>
+      <c r="X63" s="1">
         <v>90</v>
-      </c>
-      <c r="L63">
-        <v>2</v>
-      </c>
-      <c r="O63" t="s">
-        <v>196</v>
-      </c>
-      <c r="P63" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R63" s="1">
-        <v>13</v>
-      </c>
-      <c r="S63" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="T63" s="1">
-        <v>18</v>
-      </c>
-      <c r="U63" s="1">
-        <v>6</v>
-      </c>
-      <c r="V63" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="W63">
-        <v>5</v>
-      </c>
-      <c r="X63" s="1">
-        <v>80</v>
       </c>
       <c r="Y63" s="3">
         <v>2.4</v>
       </c>
       <c r="Z63">
-        <v>145.5</v>
+        <v>128.6</v>
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>5.4</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <v>7</v>
+      </c>
+      <c r="I64" t="s">
+        <v>29</v>
+      </c>
+      <c r="J64">
+        <v>6.8</v>
+      </c>
+      <c r="K64">
+        <v>5</v>
+      </c>
+      <c r="L64">
+        <v>3</v>
+      </c>
+      <c r="O64" t="s">
+        <v>194</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R64" s="1">
         <v>15</v>
       </c>
-      <c r="B64" t="s">
-        <v>195</v>
-      </c>
-      <c r="C64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64">
-        <v>5</v>
-      </c>
-      <c r="F64">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G64">
-        <v>3</v>
-      </c>
-      <c r="H64">
+      <c r="S64" s="1">
         <v>4</v>
       </c>
-      <c r="I64" t="s">
-        <v>35</v>
-      </c>
-      <c r="J64">
-        <v>11.5</v>
-      </c>
-      <c r="K64">
-        <v>50</v>
-      </c>
-      <c r="L64">
-        <v>1.9</v>
-      </c>
-      <c r="O64" t="s">
-        <v>53</v>
-      </c>
-      <c r="P64" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q64" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R64" s="1">
-        <v>14</v>
-      </c>
-      <c r="S64" s="1">
-        <v>1</v>
-      </c>
       <c r="T64" s="1">
-        <v>24</v>
+        <v>16.5</v>
       </c>
       <c r="U64" s="1">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="V64" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W64">
-        <v>2.8E-3</v>
+        <v>9</v>
       </c>
       <c r="X64" s="1">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="Y64" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="Z64">
-        <v>50</v>
+        <v>257.10000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>5.6</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <v>7</v>
+      </c>
+      <c r="I65" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65">
+        <v>3.3</v>
+      </c>
+      <c r="K65">
+        <v>90</v>
+      </c>
+      <c r="L65">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O65" t="s">
+        <v>195</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q65" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E65">
-        <v>5</v>
-      </c>
-      <c r="F65">
-        <v>4.8</v>
-      </c>
-      <c r="G65">
-        <v>2</v>
-      </c>
-      <c r="H65">
-        <v>6</v>
-      </c>
-      <c r="I65" t="s">
-        <v>35</v>
-      </c>
-      <c r="J65">
-        <v>5</v>
-      </c>
-      <c r="K65">
-        <v>80</v>
-      </c>
-      <c r="L65">
-        <v>2.4</v>
-      </c>
-      <c r="O65" t="s">
-        <v>54</v>
-      </c>
-      <c r="P65" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q65" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="R65" s="1">
         <v>15</v>
       </c>
       <c r="S65" s="1">
-        <v>1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="T65" s="1">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="U65" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="V65" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W65">
         <v>10</v>
       </c>
       <c r="X65" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="Y65" s="3">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="Z65">
-        <v>16.7</v>
+        <v>156.30000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D66" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66">
+        <v>4</v>
+      </c>
+      <c r="G66">
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <v>5.5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66">
+        <v>9.5</v>
+      </c>
+      <c r="K66">
+        <v>90</v>
+      </c>
+      <c r="L66">
+        <v>2</v>
+      </c>
+      <c r="O66" t="s">
+        <v>196</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R66" s="1">
+        <v>15</v>
+      </c>
+      <c r="S66" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="T66" s="1">
+        <v>18</v>
+      </c>
+      <c r="U66" s="1">
         <v>6</v>
       </c>
-      <c r="F66">
-        <v>3</v>
-      </c>
-      <c r="G66">
+      <c r="V66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="W66">
         <v>5</v>
       </c>
-      <c r="H66">
-        <v>3</v>
-      </c>
-      <c r="I66" t="s">
-        <v>40</v>
-      </c>
-      <c r="J66">
-        <v>53</v>
-      </c>
-      <c r="K66">
-        <v>100</v>
-      </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-      <c r="O66" t="s">
-        <v>197</v>
-      </c>
-      <c r="P66" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q66" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R66" s="1">
-        <v>16</v>
-      </c>
-      <c r="S66" s="1">
-        <v>3</v>
-      </c>
-      <c r="T66" s="1">
-        <v>9</v>
-      </c>
-      <c r="U66" s="1">
-        <v>3</v>
-      </c>
-      <c r="V66" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="W66">
-        <v>53</v>
-      </c>
       <c r="X66" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Y66" s="3">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="Z66">
-        <v>0</v>
+        <v>145.5</v>
       </c>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C67" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D67" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E67">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67">
-        <v>3.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
         <v>4</v>
       </c>
-      <c r="H67">
-        <v>5</v>
-      </c>
       <c r="I67" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J67">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="K67">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="L67">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="O67" t="s">
-        <v>198</v>
+        <v>53</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="R67" s="1">
         <v>16</v>
       </c>
       <c r="S67" s="1">
-        <v>3.4</v>
+        <v>1</v>
       </c>
       <c r="T67" s="1">
+        <v>24</v>
+      </c>
+      <c r="U67" s="1">
+        <v>8</v>
+      </c>
+      <c r="V67" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="W67">
+        <v>2.8E-3</v>
+      </c>
+      <c r="X67" s="1">
         <v>15</v>
       </c>
-      <c r="U67" s="1">
-        <v>5</v>
-      </c>
-      <c r="V67" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="W67">
-        <v>11</v>
-      </c>
-      <c r="X67" s="1">
-        <v>90</v>
-      </c>
       <c r="Y67" s="3">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z67">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C68" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E68">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="G68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H68">
         <v>6</v>
       </c>
       <c r="I68" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J68">
-        <v>2.2999999999999998</v>
+        <v>5</v>
       </c>
       <c r="K68">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="L68">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="O68" t="s">
-        <v>199</v>
+        <v>54</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="R68" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S68" s="1">
-        <v>3.8</v>
+        <v>1</v>
       </c>
       <c r="T68" s="1">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="U68" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="V68" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W68">
-        <v>2.2999999999999998</v>
+        <v>10</v>
       </c>
       <c r="X68" s="1">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="Y68" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z68">
-        <v>0</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C69" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H69">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I69" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J69">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="K69">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="L69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O69" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="R69" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S69" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T69" s="1">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="U69" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="W69">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="X69" s="1">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="Y69" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z69">
-        <v>466.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>46</v>
+        <v>198</v>
       </c>
       <c r="C70" t="s">
-        <v>201</v>
+        <v>41</v>
       </c>
       <c r="D70" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E70">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I70" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J70">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="K70">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L70">
         <v>1</v>
       </c>
       <c r="O70" t="s">
-        <v>55</v>
+        <v>198</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="R70" s="1">
         <v>18</v>
       </c>
       <c r="S70" s="1">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="T70" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="U70" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V70" s="1" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="W70">
-        <v>60</v>
+        <v>11</v>
+      </c>
+      <c r="X70" s="1">
+        <v>90</v>
       </c>
       <c r="Y70" s="3">
         <v>1</v>
@@ -4949,72 +4886,367 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D71" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E71">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F71">
-        <v>1.1000000000000001</v>
+        <v>3.8</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H71">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I71" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J71">
-        <v>60</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K71">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="L71">
         <v>1</v>
       </c>
       <c r="O71" t="s">
-        <v>56</v>
+        <v>199</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="R71" s="1">
         <v>18</v>
       </c>
       <c r="S71" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="T71" s="1">
+        <v>18</v>
+      </c>
+      <c r="U71" s="1">
+        <v>6</v>
+      </c>
+      <c r="V71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W71">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X71" s="1">
+        <v>110</v>
+      </c>
+      <c r="Y71" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" t="s">
+        <v>44</v>
+      </c>
+      <c r="E72">
+        <v>7</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72">
+        <v>8</v>
+      </c>
+      <c r="I72" t="s">
+        <v>45</v>
+      </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
+      <c r="K72">
+        <v>140</v>
+      </c>
+      <c r="L72">
+        <v>2</v>
+      </c>
+      <c r="O72" t="s">
+        <v>200</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R72" s="1">
+        <v>19</v>
+      </c>
+      <c r="S72" s="1">
+        <v>2</v>
+      </c>
+      <c r="T72" s="1">
+        <v>24</v>
+      </c>
+      <c r="U72" s="1">
+        <v>8</v>
+      </c>
+      <c r="V72" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W72">
+        <v>4</v>
+      </c>
+      <c r="X72" s="1">
+        <v>140</v>
+      </c>
+      <c r="Y72" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z72">
+        <v>466.7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="O73" t="s">
+        <v>211</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="R73" s="1">
+        <v>20</v>
+      </c>
+      <c r="S73" s="1">
+        <v>2</v>
+      </c>
+      <c r="T73" s="1">
+        <v>24</v>
+      </c>
+      <c r="U73" s="1">
+        <v>8</v>
+      </c>
+      <c r="V73" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="W73" s="1">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="X73" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="Y73" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="O74" t="s">
+        <v>212</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="R74" s="1">
+        <v>20</v>
+      </c>
+      <c r="S74" s="1">
+        <v>2</v>
+      </c>
+      <c r="T74" s="1">
+        <v>24</v>
+      </c>
+      <c r="U74" s="1">
+        <v>8</v>
+      </c>
+      <c r="V74" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="W74" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="X74" s="1">
+        <v>43</v>
+      </c>
+      <c r="Y74" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>21</v>
+      </c>
+      <c r="B75" t="s">
+        <v>46</v>
+      </c>
+      <c r="C75" t="s">
+        <v>201</v>
+      </c>
+      <c r="D75" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75">
+        <v>8</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75" t="s">
+        <v>48</v>
+      </c>
+      <c r="J75">
+        <v>60</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="O75" t="s">
+        <v>55</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R75" s="1">
+        <v>21</v>
+      </c>
+      <c r="S75" s="1">
+        <v>1</v>
+      </c>
+      <c r="T75" s="1">
+        <v>6</v>
+      </c>
+      <c r="U75" s="1">
+        <v>2</v>
+      </c>
+      <c r="V75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W75">
+        <v>60</v>
+      </c>
+      <c r="Y75" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>22</v>
+      </c>
+      <c r="B76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C76" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" t="s">
+        <v>47</v>
+      </c>
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T71" s="1">
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>8</v>
+      </c>
+      <c r="I76" t="s">
+        <v>48</v>
+      </c>
+      <c r="J76">
+        <v>60</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="O76" t="s">
+        <v>56</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R76" s="1">
+        <v>21</v>
+      </c>
+      <c r="S76" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T76" s="1">
         <v>24</v>
       </c>
-      <c r="U71" s="1">
-        <v>8</v>
-      </c>
-      <c r="V71" s="1" t="s">
+      <c r="U76" s="1">
+        <v>8</v>
+      </c>
+      <c r="V76" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W71">
+      <c r="W76">
         <v>60</v>
       </c>
-      <c r="Y71" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z71">
+      <c r="Y76" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z76">
         <v>0</v>
       </c>
     </row>

</xml_diff>